<commit_message>
cambios en la basede datos, se añade tabla tipo:usuarios
</commit_message>
<xml_diff>
--- a/documentacion/primer sprint/docsprint1.xlsx
+++ b/documentacion/primer sprint/docsprint1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="productBack" sheetId="3" r:id="rId3"/>
     <sheet name="ProducBack-1" sheetId="4" r:id="rId4"/>
     <sheet name="sprint1.1" sheetId="5" r:id="rId5"/>
+    <sheet name="sprint2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="149">
   <si>
     <t>TAREAS</t>
   </si>
@@ -470,6 +471,54 @@
 de venta, precio de 
 compra, si el producto 
 tiene algún descuento.</t>
+  </si>
+  <si>
+    <t>Eliminar venta.</t>
+  </si>
+  <si>
+    <t>Modificar venta.</t>
+  </si>
+  <si>
+    <t>Diseñar la base de datos con las tablas</t>
+  </si>
+  <si>
+    <t>Diseñar prototipo de IU para registro</t>
+  </si>
+  <si>
+    <t>de venta.</t>
+  </si>
+  <si>
+    <t>Diseñar prototipo de IU paraModificar</t>
+  </si>
+  <si>
+    <t>venta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diseño prototipo de IU para eliminar </t>
+  </si>
+  <si>
+    <t>Yo como administrador  necesito registrar, modificar, eliminar cada producto vendido de tal manera que  disminuya el stock de la tienda.</t>
+  </si>
+  <si>
+    <t>Autenticación</t>
+  </si>
+  <si>
+    <t>Yo como usuario (administrador y vendedor) debo autenticar mi contraseña y nombre  para poder  ingresar a mi cuenta</t>
+  </si>
+  <si>
+    <t>Yo como usuario(administra-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trador y vendedor)debo </t>
+  </si>
+  <si>
+    <t>autentificar mi contraseña y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre de usuario para </t>
+  </si>
+  <si>
+    <t>poder ingresar a mi cuenta.</t>
   </si>
 </sst>
 </file>
@@ -525,13 +574,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -827,237 +876,179 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1065,12 +1056,87 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66CCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1626,13 +1692,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1652,16 +1718,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="30">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="30">
         <v>20</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="30">
         <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1669,10 +1735,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="6" t="s">
         <v>74</v>
       </c>
@@ -1708,16 +1774,16 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
+      <c r="A7" s="30">
         <v>4</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="30">
         <v>13</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="30">
         <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1725,52 +1791,52 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25">
+      <c r="A12" s="30">
         <v>5</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="30">
         <v>13</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="30">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -1778,52 +1844,52 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25">
+      <c r="A17" s="30">
         <v>6</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="30">
         <v>8</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="30">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -1831,52 +1897,52 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25">
+      <c r="A22" s="30">
         <v>7</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="30">
         <v>8</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="30">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -1884,52 +1950,52 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25">
+      <c r="A27" s="30">
         <v>8</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="30">
         <v>5</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="30">
         <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -1937,112 +2003,112 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25">
+      <c r="A32" s="30">
         <v>9</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="25">
+      <c r="C32" s="30">
         <v>5</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="30">
         <v>1</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="28"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25">
+      <c r="A38" s="30">
         <v>10</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="25">
+      <c r="C38" s="30">
         <v>5</v>
       </c>
-      <c r="D38" s="25">
+      <c r="D38" s="30">
         <v>1</v>
       </c>
       <c r="E38" s="6" t="s">
@@ -2050,37 +2116,37 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
       <c r="E39" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
       <c r="E42" s="9" t="s">
         <v>84</v>
       </c>
@@ -2105,19 +2171,11 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A42"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="B32:B37"/>
@@ -2134,11 +2192,19 @@
     <mergeCell ref="D7:D11"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2150,7 +2216,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,11 +2226,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2424,34 +2490,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="109" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G2" t="s">
@@ -2459,16 +2525,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="106">
+      <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="105">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="27">
         <v>1</v>
       </c>
       <c r="G3">
@@ -2476,16 +2542,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="116">
+      <c r="A4" s="94">
         <v>2</v>
       </c>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="95" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="120">
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="98">
         <v>1</v>
       </c>
       <c r="G4">
@@ -2493,16 +2559,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="106">
+      <c r="A5" s="28">
         <v>3</v>
       </c>
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="105">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="27">
         <v>1</v>
       </c>
       <c r="G5">
@@ -2510,16 +2576,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="116">
+      <c r="A6" s="94">
         <v>4</v>
       </c>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="95" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="120">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98">
         <v>1</v>
       </c>
       <c r="G6">
@@ -2527,124 +2593,119 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="106">
+      <c r="A7" s="28">
         <v>5</v>
       </c>
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="105">
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="116">
+      <c r="A8" s="94">
         <v>6</v>
       </c>
-      <c r="B8" s="117" t="s">
+      <c r="B8" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="120">
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="98">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="106">
+      <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="110" t="s">
+      <c r="B9" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="105">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="116">
+      <c r="A10" s="94">
         <v>8</v>
       </c>
-      <c r="B10" s="117" t="s">
+      <c r="B10" s="95" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
-      <c r="E10" s="119"/>
-      <c r="F10" s="120">
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="106">
+      <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="105">
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="116">
+      <c r="A12" s="94">
         <v>11</v>
       </c>
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="119"/>
-      <c r="F12" s="120">
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="98">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="106">
+      <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="110" t="s">
+      <c r="B13" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="105">
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="116">
+      <c r="A14" s="94">
         <v>14</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="120">
+      <c r="C14" s="96"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="98">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A1:F1"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B12:E12"/>
@@ -2654,6 +2715,11 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2664,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2677,359 +2743,560 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="102"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="89" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="101"/>
-      <c r="H2" s="102"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="101"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="50">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="88"/>
       <c r="D3" s="50">
         <v>13</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="82" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="84"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="105"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="51"/>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="51"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="32" t="s">
+      <c r="E4" s="54"/>
+      <c r="F4" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="86"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
       <c r="D5" s="51"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="82" t="s">
+      <c r="E5" s="54"/>
+      <c r="F5" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="83"/>
-      <c r="H5" s="84"/>
-      <c r="J5" s="49"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="105"/>
+      <c r="J5" s="26"/>
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="60"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="77"/>
       <c r="D6" s="51"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="41" t="s">
+      <c r="E6" s="54"/>
+      <c r="F6" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="67"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="77"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="45"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="70"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="51"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="51"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="85" t="s">
+      <c r="E9" s="54"/>
+      <c r="F9" s="106" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="87"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="108"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="51"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="90"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="111"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="51"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="35" t="s">
+      <c r="E11" s="54"/>
+      <c r="F11" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="81"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="51"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="60"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="51"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="84"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="51"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="85" t="s">
+      <c r="E13" s="54"/>
+      <c r="F13" s="106" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="86"/>
-      <c r="H13" s="87"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="108"/>
     </row>
     <row r="14" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="62"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="52"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="90"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="111"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="50">
         <v>13</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="66" t="s">
+      <c r="E15" s="53"/>
+      <c r="F15" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="67"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="51"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="69"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="61"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="77"/>
       <c r="D17" s="51"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="72"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="64"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="51"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="91" t="s">
+      <c r="E18" s="54"/>
+      <c r="F18" s="112" t="s">
         <v>127</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="93"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="114"/>
       <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="60"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="51"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="96"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="117"/>
       <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="77"/>
       <c r="D20" s="51"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="76" t="s">
+      <c r="E20" s="54"/>
+      <c r="F20" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="77"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="30"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="25"/>
     </row>
     <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="51"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="30"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="51"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="60"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="77"/>
       <c r="D22" s="51"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="91" t="s">
+      <c r="E22" s="54"/>
+      <c r="F22" s="112" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="92"/>
-      <c r="H22" s="93"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="114"/>
       <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="51"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="60"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="77"/>
       <c r="D23" s="51"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="96"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="117"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="51"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="60"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="77"/>
       <c r="D24" s="51"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="73" t="s">
+      <c r="E24" s="54"/>
+      <c r="F24" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="74"/>
-      <c r="H24" s="75"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="51"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="60"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="51"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="97" t="s">
+      <c r="E25" s="54"/>
+      <c r="F25" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="98"/>
-      <c r="H25" s="99"/>
+      <c r="G25" s="119"/>
+      <c r="H25" s="120"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="52"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="79"/>
       <c r="D26" s="52"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="73" t="s">
+      <c r="E26" s="55"/>
+      <c r="F26" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="74"/>
-      <c r="H26" s="75"/>
+      <c r="G26" s="119"/>
+      <c r="H26" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F20:H21"/>
-    <mergeCell ref="F22:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="D15:D26"/>
-    <mergeCell ref="E15:E26"/>
-    <mergeCell ref="F15:H17"/>
-    <mergeCell ref="F18:H19"/>
     <mergeCell ref="E3:E14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="F9:H10"/>
     <mergeCell ref="F6:H8"/>
     <mergeCell ref="A3:A14"/>
-    <mergeCell ref="B16:C26"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F11:H12"/>
     <mergeCell ref="F13:H14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B4:C14"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="D3:D14"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="D15:D26"/>
+    <mergeCell ref="E15:E26"/>
+    <mergeCell ref="F15:H17"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="B16:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="F22:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="102" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="102" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="99" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="100"/>
+      <c r="H2" s="101"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="121">
+        <v>1</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="F3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="122"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="122"/>
+      <c r="B5" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="124"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="122"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="F6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="122"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="F7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="122"/>
+      <c r="B8" s="124"/>
+      <c r="C8" s="124"/>
+      <c r="F8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="122"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="124"/>
+      <c r="F9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="122"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
+      <c r="F10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="122"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="124"/>
+      <c r="F11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="122"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="124"/>
+      <c r="F12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="122"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
+      <c r="F13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B5:C13"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="B3:C4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cambios en la interfaz de venta
</commit_message>
<xml_diff>
--- a/documentacion/primer sprint/docsprint1.xlsx
+++ b/documentacion/primer sprint/docsprint1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="153">
   <si>
     <t>TAREAS</t>
   </si>
@@ -519,6 +519,18 @@
   </si>
   <si>
     <t>poder ingresar a mi cuenta.</t>
+  </si>
+  <si>
+    <t>Realizar la implementacion de la funcionaliadad para registrar ventas en la BD.</t>
+  </si>
+  <si>
+    <t>Diseñar la IU para relizar la autenticacion</t>
+  </si>
+  <si>
+    <t>Realizar la implemetacion del metodo que permita verificar los datos del usuario en BD.</t>
+  </si>
+  <si>
+    <t>Diseñar la pagina de inicio para usuarios autenticados.</t>
   </si>
 </sst>
 </file>
@@ -885,92 +897,70 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -999,9 +989,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1017,75 +1033,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1105,6 +1090,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1114,6 +1126,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1122,9 +1137,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1692,13 +1704,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1718,16 +1730,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="34">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="34">
         <v>20</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="34">
         <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -1735,10 +1747,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="6" t="s">
         <v>74</v>
       </c>
@@ -1774,16 +1786,16 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
+      <c r="A7" s="34">
         <v>4</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="34">
         <v>13</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="34">
         <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -1791,52 +1803,52 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="34">
         <v>5</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="34">
         <v>13</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="34">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -1844,52 +1856,52 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="A17" s="34">
         <v>6</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="34">
         <v>8</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="34">
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -1897,52 +1909,52 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="9" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="34">
         <v>7</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="34">
         <v>8</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="34">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -1950,52 +1962,52 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30">
+      <c r="A27" s="34">
         <v>8</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="34">
         <v>5</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D27" s="34">
         <v>1</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -2003,112 +2015,112 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30">
+      <c r="A32" s="34">
         <v>9</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="30">
+      <c r="C32" s="34">
         <v>5</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="34">
         <v>1</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="37" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="37"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
       <c r="E35" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
       <c r="E36" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
       <c r="E37" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30">
+      <c r="A38" s="34">
         <v>10</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C38" s="34">
         <v>5</v>
       </c>
-      <c r="D38" s="30">
+      <c r="D38" s="34">
         <v>1</v>
       </c>
       <c r="E38" s="6" t="s">
@@ -2116,37 +2128,37 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
       <c r="E41" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
       <c r="E42" s="9" t="s">
         <v>84</v>
       </c>
@@ -2171,11 +2183,19 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="B32:B37"/>
@@ -2192,19 +2212,11 @@
     <mergeCell ref="D7:D11"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2226,11 +2238,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2497,26 +2509,26 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
       <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="29" t="s">
         <v>117</v>
       </c>
@@ -2528,12 +2540,12 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="48"/>
       <c r="F3" s="27">
         <v>1</v>
       </c>
@@ -2542,16 +2554,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="94">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="98">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="32">
         <v>1</v>
       </c>
       <c r="G4">
@@ -2562,12 +2574,12 @@
       <c r="A5" s="28">
         <v>3</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="27">
         <v>1</v>
       </c>
@@ -2576,16 +2588,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="94">
+      <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="98">
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="32">
         <v>1</v>
       </c>
       <c r="G6">
@@ -2596,27 +2608,27 @@
       <c r="A7" s="28">
         <v>5</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="94">
+      <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="98">
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="32">
         <v>2</v>
       </c>
     </row>
@@ -2624,27 +2636,27 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="94">
+      <c r="A10" s="31">
         <v>8</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="98">
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="32">
         <v>2</v>
       </c>
     </row>
@@ -2652,27 +2664,27 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="94">
+      <c r="A12" s="31">
         <v>11</v>
       </c>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="98">
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="32">
         <v>3</v>
       </c>
     </row>
@@ -2680,32 +2692,37 @@
       <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="94">
+      <c r="A14" s="31">
         <v>14</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="98">
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="32">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B12:E12"/>
@@ -2715,11 +2732,6 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2743,310 +2755,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="101"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="102" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="99" t="s">
+      <c r="F2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="100"/>
-      <c r="H2" s="101"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="50">
+      <c r="A3" s="70">
         <v>1</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="50">
+      <c r="C3" s="87"/>
+      <c r="D3" s="70">
         <v>13</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="103" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="104"/>
-      <c r="H3" s="105"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="90"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="74" t="s">
+      <c r="A4" s="71"/>
+      <c r="B4" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="85" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="91"/>
-      <c r="H4" s="86"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="103" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="104"/>
-      <c r="H5" s="105"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="90"/>
       <c r="J5" s="26"/>
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="65" t="s">
+      <c r="A6" s="71"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="66"/>
-      <c r="H6" s="67"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="70"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="73"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="69"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="106" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="107"/>
-      <c r="H9" s="108"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="111"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="60"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="74" t="s">
+      <c r="A11" s="71"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="80"/>
-      <c r="H11" s="81"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="77"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="84"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="80"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="106" t="s">
+      <c r="A13" s="71"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="107"/>
-      <c r="H13" s="108"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="111"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="60"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="50">
+      <c r="A15" s="70">
         <v>2</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="50">
+      <c r="C15" s="93"/>
+      <c r="D15" s="70">
         <v>13</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="56" t="s">
+      <c r="E15" s="49"/>
+      <c r="F15" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="57"/>
-      <c r="H15" s="58"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="96"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="74" t="s">
+      <c r="A16" s="71"/>
+      <c r="B16" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="61"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="99"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="64"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="102"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="112" t="s">
+      <c r="A18" s="71"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="G18" s="113"/>
-      <c r="H18" s="114"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="105"/>
       <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="117"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="108"/>
       <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="41" t="s">
+      <c r="A20" s="71"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="43"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="111"/>
       <c r="I20" s="25"/>
     </row>
     <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="76"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="46"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="114"/>
       <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="112" t="s">
+      <c r="A22" s="71"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="103" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="113"/>
-      <c r="H22" s="114"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="105"/>
       <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
-      <c r="B23" s="76"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="115"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="117"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="108"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="51"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="47" t="s">
+      <c r="A24" s="71"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="48"/>
-      <c r="H24" s="49"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="117"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="51"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="54"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="118" t="s">
         <v>129</v>
       </c>
@@ -3054,11 +3066,11 @@
       <c r="H25" s="120"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="78"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="55"/>
+      <c r="A26" s="72"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="118" t="s">
         <v>130</v>
       </c>
@@ -3067,6 +3079,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="D15:D26"/>
+    <mergeCell ref="E15:E26"/>
+    <mergeCell ref="F15:H17"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="B16:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="F22:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
     <mergeCell ref="E3:E14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:H2"/>
@@ -3082,18 +3106,6 @@
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="D3:D14"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="D15:D26"/>
-    <mergeCell ref="E15:E26"/>
-    <mergeCell ref="F15:H17"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="B16:C26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F20:H21"/>
-    <mergeCell ref="F22:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3105,7 +3117,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,63 +3129,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="101"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="102" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="99" t="s">
+      <c r="F2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="100"/>
-      <c r="H2" s="101"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="121">
+      <c r="A3" s="122">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="95" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="57"/>
+      <c r="C3" s="95"/>
       <c r="F3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122"/>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="122"/>
-      <c r="B5" s="124" t="s">
+      <c r="A5" s="123"/>
+      <c r="B5" s="121" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="124"/>
+      <c r="C5" s="121"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="23" t="s">
+        <v>149</v>
+      </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
@@ -3182,65 +3196,65 @@
       <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="122"/>
-      <c r="B6" s="124"/>
-      <c r="C6" s="124"/>
+      <c r="A6" s="123"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
       <c r="F6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
+      <c r="A7" s="123"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121"/>
       <c r="F7" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
-      <c r="B8" s="124"/>
-      <c r="C8" s="124"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="121"/>
       <c r="F8" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="124"/>
-      <c r="C9" s="124"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="121"/>
       <c r="F9" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
-      <c r="B10" s="124"/>
-      <c r="C10" s="124"/>
+      <c r="A10" s="123"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="121"/>
       <c r="F10" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
-      <c r="B11" s="124"/>
-      <c r="C11" s="124"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
       <c r="F11" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="124"/>
-      <c r="C12" s="124"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
       <c r="F12" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="124"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="121"/>
       <c r="F13" t="s">
         <v>139</v>
       </c>
@@ -3252,15 +3266,24 @@
       <c r="B14" t="s">
         <v>142</v>
       </c>
+      <c r="F14" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>144</v>
       </c>
+      <c r="F15" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>145</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se modifico la iu de listar productos y modificar productos
</commit_message>
<xml_diff>
--- a/documentacion/primer sprint/docsprint1.xlsx
+++ b/documentacion/primer sprint/docsprint1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="154">
   <si>
     <t>TAREAS</t>
   </si>
@@ -531,6 +531,9 @@
   </si>
   <si>
     <t>Diseñar la pagina de inicio para usuarios autenticados.</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
   </si>
 </sst>
 </file>
@@ -908,33 +911,143 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -989,20 +1102,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1017,21 +1118,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1042,90 +1128,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1704,13 +1707,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1733,7 +1736,7 @@
       <c r="A3" s="34">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="34">
@@ -1748,7 +1751,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
-      <c r="B4" s="37"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="6" t="s">
@@ -1789,7 +1792,7 @@
       <c r="A7" s="34">
         <v>4</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="36" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="34">
@@ -1804,7 +1807,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
-      <c r="B8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="6" t="s">
@@ -1813,7 +1816,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
-      <c r="B9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="6" t="s">
@@ -1822,7 +1825,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
-      <c r="B10" s="38"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="6" t="s">
@@ -1831,7 +1834,7 @@
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
-      <c r="B11" s="38"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
       <c r="E11" s="9" t="s">
@@ -1842,7 +1845,7 @@
       <c r="A12" s="34">
         <v>5</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="36" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="34">
@@ -1857,7 +1860,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
-      <c r="B13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="6" t="s">
@@ -1866,7 +1869,7 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="34"/>
-      <c r="B14" s="38"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
       <c r="E14" s="6" t="s">
@@ -1875,7 +1878,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
-      <c r="B15" s="38"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
       <c r="E15" s="6" t="s">
@@ -1884,7 +1887,7 @@
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
-      <c r="B16" s="38"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
       <c r="E16" s="9" t="s">
@@ -1895,7 +1898,7 @@
       <c r="A17" s="34">
         <v>6</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="36" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="34">
@@ -1910,7 +1913,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
-      <c r="B18" s="38"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
       <c r="E18" s="6" t="s">
@@ -1919,7 +1922,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
-      <c r="B19" s="38"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="6" t="s">
@@ -1928,7 +1931,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
-      <c r="B20" s="38"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="34"/>
       <c r="D20" s="34"/>
       <c r="E20" s="6" t="s">
@@ -1937,7 +1940,7 @@
     </row>
     <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="34"/>
-      <c r="B21" s="38"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="9" t="s">
@@ -1948,7 +1951,7 @@
       <c r="A22" s="34">
         <v>7</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="36" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="34">
@@ -2001,7 +2004,7 @@
       <c r="A27" s="34">
         <v>8</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="36" t="s">
         <v>64</v>
       </c>
       <c r="C27" s="34">
@@ -2016,7 +2019,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
-      <c r="B28" s="38"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
       <c r="E28" s="6" t="s">
@@ -2025,7 +2028,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
-      <c r="B29" s="38"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="34"/>
       <c r="D29" s="34"/>
       <c r="E29" s="6" t="s">
@@ -2034,7 +2037,7 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
-      <c r="B30" s="38"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="34"/>
       <c r="D30" s="34"/>
       <c r="E30" s="6" t="s">
@@ -2043,7 +2046,7 @@
     </row>
     <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
-      <c r="B31" s="38"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="34"/>
       <c r="D31" s="34"/>
       <c r="E31" s="9" t="s">
@@ -2054,7 +2057,7 @@
       <c r="A32" s="34">
         <v>9</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="36" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="34">
@@ -2063,20 +2066,20 @@
       <c r="D32" s="34">
         <v>1</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="35" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="34"/>
-      <c r="B33" s="38"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="34"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="37"/>
+      <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
-      <c r="B34" s="38"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="34"/>
       <c r="D34" s="34"/>
       <c r="E34" s="6" t="s">
@@ -2085,7 +2088,7 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
-      <c r="B35" s="38"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="34"/>
       <c r="D35" s="34"/>
       <c r="E35" s="6" t="s">
@@ -2094,7 +2097,7 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
-      <c r="B36" s="38"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
       <c r="E36" s="6" t="s">
@@ -2103,7 +2106,7 @@
     </row>
     <row r="37" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
-      <c r="B37" s="38"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="34"/>
       <c r="D37" s="34"/>
       <c r="E37" s="9" t="s">
@@ -2114,7 +2117,7 @@
       <c r="A38" s="34">
         <v>10</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="36" t="s">
         <v>66</v>
       </c>
       <c r="C38" s="34">
@@ -2129,7 +2132,7 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
-      <c r="B39" s="38"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="6" t="s">
@@ -2138,7 +2141,7 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
-      <c r="B40" s="38"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
       <c r="E40" s="6" t="s">
@@ -2147,7 +2150,7 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="34"/>
-      <c r="B41" s="38"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="34"/>
       <c r="D41" s="34"/>
       <c r="E41" s="6" t="s">
@@ -2156,7 +2159,7 @@
     </row>
     <row r="42" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
-      <c r="B42" s="38"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="34"/>
       <c r="D42" s="34"/>
       <c r="E42" s="9" t="s">
@@ -2183,19 +2186,11 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A42"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="B32:B37"/>
@@ -2212,11 +2207,19 @@
     <mergeCell ref="D7:D11"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2238,11 +2241,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2509,26 +2512,26 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
       <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="29" t="s">
         <v>117</v>
       </c>
@@ -2557,12 +2560,12 @@
       <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="44"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="32">
         <v>1</v>
       </c>
@@ -2574,12 +2577,12 @@
       <c r="A5" s="28">
         <v>3</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
       <c r="F5" s="27">
         <v>1</v>
       </c>
@@ -2591,12 +2594,12 @@
       <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="32">
         <v>1</v>
       </c>
@@ -2608,12 +2611,12 @@
       <c r="A7" s="28">
         <v>5</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="27">
         <v>2</v>
       </c>
@@ -2622,12 +2625,12 @@
       <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="32">
         <v>2</v>
       </c>
@@ -2636,12 +2639,12 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="27">
         <v>2</v>
       </c>
@@ -2650,12 +2653,12 @@
       <c r="A10" s="31">
         <v>8</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="44"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="32">
         <v>2</v>
       </c>
@@ -2664,12 +2667,12 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="27">
         <v>3</v>
       </c>
@@ -2678,12 +2681,12 @@
       <c r="A12" s="31">
         <v>11</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="32">
         <v>3</v>
       </c>
@@ -2692,12 +2695,12 @@
       <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="27">
         <v>4</v>
       </c>
@@ -2706,23 +2709,18 @@
       <c r="A14" s="31">
         <v>14</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="32">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A1:F1"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B12:E12"/>
@@ -2732,6 +2730,11 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2742,8 +2745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,342 +2758,330 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="92"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="109"/>
       <c r="D2" s="33" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="70">
+      <c r="A3" s="49">
         <v>1</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="115" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="70">
+      <c r="C3" s="116"/>
+      <c r="D3" s="49">
         <v>13</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="88" t="s">
+      <c r="E3" s="52"/>
+      <c r="F3" s="117" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="119"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="71"/>
-      <c r="B4" s="75" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="70" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="91" t="s">
+      <c r="C4" s="71"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="93"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="88" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="117" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="89"/>
-      <c r="H5" s="90"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="119"/>
       <c r="J5" s="26"/>
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="61" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="99" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="62"/>
-      <c r="H6" s="63"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="101"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="66"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="104"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="69"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="107"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="55" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="56"/>
-      <c r="H9" s="57"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="95"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="82"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="60"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="98"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="75" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="76"/>
-      <c r="H11" s="77"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="111"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="114"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="55" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="93" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="57"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="95"/>
     </row>
     <row r="14" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="85"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="98"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="70">
+      <c r="A15" s="49">
         <v>2</v>
       </c>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="93"/>
-      <c r="D15" s="70">
+      <c r="C15" s="77"/>
+      <c r="D15" s="49">
         <v>13</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="94" t="s">
+      <c r="E15" s="52"/>
+      <c r="F15" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="95"/>
-      <c r="H15" s="96"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="57"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
-      <c r="B16" s="75" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="99"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="60"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="102"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="63"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="103" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="G18" s="104"/>
-      <c r="H18" s="105"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="66"/>
       <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="108"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="69"/>
       <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="109" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="110"/>
-      <c r="H20" s="111"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="80"/>
       <c r="I20" s="25"/>
     </row>
     <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="71"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="113"/>
-      <c r="H21" s="114"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="83"/>
       <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="103" t="s">
+      <c r="A22" s="50"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="104"/>
-      <c r="H22" s="105"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="66"/>
       <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="107"/>
-      <c r="H23" s="108"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="69"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
-      <c r="B24" s="82"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="115" t="s">
+      <c r="A24" s="50"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="84" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="116"/>
-      <c r="H24" s="117"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="86"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="118" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="87" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="119"/>
-      <c r="H25" s="120"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="89"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="72"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="118" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="119"/>
-      <c r="H26" s="120"/>
+      <c r="G26" s="88"/>
+      <c r="H26" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="D15:D26"/>
-    <mergeCell ref="E15:E26"/>
-    <mergeCell ref="F15:H17"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="B16:C26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F20:H21"/>
-    <mergeCell ref="F22:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
     <mergeCell ref="E3:E14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:H2"/>
@@ -3106,6 +3097,18 @@
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="D3:D14"/>
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="D15:D26"/>
+    <mergeCell ref="E15:E26"/>
+    <mergeCell ref="F15:H17"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="B16:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="F22:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3117,7 +3120,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,45 +3132,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="92"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="108" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="109"/>
       <c r="D2" s="33" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="122">
         <v>1</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="95"/>
+      <c r="C3" s="56"/>
       <c r="F3" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
se realizo parte del sprint3
</commit_message>
<xml_diff>
--- a/documentacion/primer sprint/docsprint1.xlsx
+++ b/documentacion/primer sprint/docsprint1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos\pymes\documentacion\primer sprint\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -13,13 +18,14 @@
     <sheet name="ProducBack-1" sheetId="4" r:id="rId4"/>
     <sheet name="sprint1.1" sheetId="5" r:id="rId5"/>
     <sheet name="sprint2" sheetId="6" r:id="rId6"/>
+    <sheet name="Sprint3" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="161">
   <si>
     <t>TAREAS</t>
   </si>
@@ -534,6 +540,27 @@
   </si>
   <si>
     <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
+  </si>
+  <si>
+    <t>Hisotoria de Usuario</t>
+  </si>
+  <si>
+    <t>Gestionar proveedores</t>
+  </si>
+  <si>
+    <t>Formulario de registro.</t>
+  </si>
+  <si>
+    <t>IU para listar proveedores, eliminar y modificar.</t>
+  </si>
+  <si>
+    <t>Formulario de registro para vendedores.</t>
+  </si>
+  <si>
+    <t>IU para listar vendedores, eliminar y modificar.</t>
   </si>
 </sst>
 </file>
@@ -911,90 +938,116 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1009,115 +1062,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1128,7 +1072,90 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1156,12 +1183,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1203,7 +1233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1238,7 +1268,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1453,7 +1483,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.140625" customWidth="1"/>
     <col min="2" max="2" width="117" customWidth="1"/>
@@ -1696,7 +1726,7 @@
       <selection activeCell="B17" sqref="B17:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
@@ -1707,13 +1737,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1736,7 +1766,7 @@
       <c r="A3" s="34">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="34">
@@ -1751,7 +1781,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="6" t="s">
@@ -1792,7 +1822,7 @@
       <c r="A7" s="34">
         <v>4</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="38" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="34">
@@ -1807,7 +1837,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
-      <c r="B8" s="36"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="6" t="s">
@@ -1816,7 +1846,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
-      <c r="B9" s="36"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="6" t="s">
@@ -1825,7 +1855,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
-      <c r="B10" s="36"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="6" t="s">
@@ -1834,7 +1864,7 @@
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
-      <c r="B11" s="36"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
       <c r="E11" s="9" t="s">
@@ -1845,7 +1875,7 @@
       <c r="A12" s="34">
         <v>5</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="38" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="34">
@@ -1860,7 +1890,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
-      <c r="B13" s="36"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="6" t="s">
@@ -1869,7 +1899,7 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="34"/>
-      <c r="B14" s="36"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
       <c r="E14" s="6" t="s">
@@ -1878,7 +1908,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
-      <c r="B15" s="36"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
       <c r="E15" s="6" t="s">
@@ -1887,7 +1917,7 @@
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
-      <c r="B16" s="36"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
       <c r="E16" s="9" t="s">
@@ -1898,7 +1928,7 @@
       <c r="A17" s="34">
         <v>6</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="38" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="34">
@@ -1913,7 +1943,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
-      <c r="B18" s="36"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
       <c r="E18" s="6" t="s">
@@ -1922,7 +1952,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
-      <c r="B19" s="36"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
       <c r="E19" s="6" t="s">
@@ -1931,7 +1961,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
-      <c r="B20" s="36"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="34"/>
       <c r="D20" s="34"/>
       <c r="E20" s="6" t="s">
@@ -1940,7 +1970,7 @@
     </row>
     <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="34"/>
-      <c r="B21" s="36"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="9" t="s">
@@ -1951,7 +1981,7 @@
       <c r="A22" s="34">
         <v>7</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="38" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="34">
@@ -2004,7 +2034,7 @@
       <c r="A27" s="34">
         <v>8</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="38" t="s">
         <v>64</v>
       </c>
       <c r="C27" s="34">
@@ -2019,7 +2049,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
-      <c r="B28" s="36"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
       <c r="E28" s="6" t="s">
@@ -2028,7 +2058,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
-      <c r="B29" s="36"/>
+      <c r="B29" s="38"/>
       <c r="C29" s="34"/>
       <c r="D29" s="34"/>
       <c r="E29" s="6" t="s">
@@ -2037,7 +2067,7 @@
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
-      <c r="B30" s="36"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="34"/>
       <c r="D30" s="34"/>
       <c r="E30" s="6" t="s">
@@ -2046,7 +2076,7 @@
     </row>
     <row r="31" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
-      <c r="B31" s="36"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="34"/>
       <c r="D31" s="34"/>
       <c r="E31" s="9" t="s">
@@ -2057,7 +2087,7 @@
       <c r="A32" s="34">
         <v>9</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="38" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="34">
@@ -2066,20 +2096,20 @@
       <c r="D32" s="34">
         <v>1</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="37" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="34"/>
-      <c r="B33" s="36"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="34"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
+      <c r="E33" s="37"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
-      <c r="B34" s="36"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="34"/>
       <c r="D34" s="34"/>
       <c r="E34" s="6" t="s">
@@ -2088,7 +2118,7 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
-      <c r="B35" s="36"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="34"/>
       <c r="D35" s="34"/>
       <c r="E35" s="6" t="s">
@@ -2097,7 +2127,7 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
-      <c r="B36" s="36"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
       <c r="E36" s="6" t="s">
@@ -2106,7 +2136,7 @@
     </row>
     <row r="37" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
-      <c r="B37" s="36"/>
+      <c r="B37" s="38"/>
       <c r="C37" s="34"/>
       <c r="D37" s="34"/>
       <c r="E37" s="9" t="s">
@@ -2117,7 +2147,7 @@
       <c r="A38" s="34">
         <v>10</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="38" t="s">
         <v>66</v>
       </c>
       <c r="C38" s="34">
@@ -2132,7 +2162,7 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
-      <c r="B39" s="36"/>
+      <c r="B39" s="38"/>
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="6" t="s">
@@ -2141,7 +2171,7 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
-      <c r="B40" s="36"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
       <c r="E40" s="6" t="s">
@@ -2150,7 +2180,7 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="34"/>
-      <c r="B41" s="36"/>
+      <c r="B41" s="38"/>
       <c r="C41" s="34"/>
       <c r="D41" s="34"/>
       <c r="E41" s="6" t="s">
@@ -2159,14 +2189,14 @@
     </row>
     <row r="42" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
-      <c r="B42" s="36"/>
+      <c r="B42" s="38"/>
       <c r="C42" s="34"/>
       <c r="D42" s="34"/>
       <c r="E42" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>11</v>
       </c>
@@ -2186,11 +2216,19 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="E32:E33"/>
     <mergeCell ref="B32:B37"/>
@@ -2207,19 +2245,11 @@
     <mergeCell ref="D7:D11"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2234,18 +2264,18 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2506,32 +2536,32 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
       <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="29" t="s">
         <v>117</v>
       </c>
@@ -2560,12 +2590,12 @@
       <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="32">
         <v>1</v>
       </c>
@@ -2577,12 +2607,12 @@
       <c r="A5" s="28">
         <v>3</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="45"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="27">
         <v>1</v>
       </c>
@@ -2594,12 +2624,12 @@
       <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="32">
         <v>1</v>
       </c>
@@ -2611,26 +2641,29 @@
       <c r="A7" s="28">
         <v>5</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="27">
         <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="32">
         <v>2</v>
       </c>
@@ -2639,12 +2672,12 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="27">
         <v>2</v>
       </c>
@@ -2653,12 +2686,12 @@
       <c r="A10" s="31">
         <v>8</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="32">
         <v>2</v>
       </c>
@@ -2667,12 +2700,12 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="27">
         <v>3</v>
       </c>
@@ -2681,13 +2714,16 @@
       <c r="A12" s="31">
         <v>11</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="32">
+        <v>3</v>
+      </c>
+      <c r="G12">
         <v>3</v>
       </c>
     </row>
@@ -2695,12 +2731,12 @@
       <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="45"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="27">
         <v>4</v>
       </c>
@@ -2709,18 +2745,23 @@
       <c r="A14" s="31">
         <v>14</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="32">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B12:E12"/>
@@ -2730,11 +2771,6 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2749,7 +2785,7 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
@@ -2758,330 +2794,342 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="109"/>
+      <c r="C2" s="74"/>
       <c r="D2" s="33" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="92"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="49">
+      <c r="A3" s="70">
         <v>1</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="116"/>
-      <c r="D3" s="49">
+      <c r="C3" s="87"/>
+      <c r="D3" s="70">
         <v>13</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="117" t="s">
+      <c r="E3" s="49"/>
+      <c r="F3" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="118"/>
-      <c r="H3" s="119"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="90"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="70" t="s">
+      <c r="A4" s="71"/>
+      <c r="B4" s="75" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="76" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="120"/>
-      <c r="H4" s="77"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="117" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="88" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="118"/>
-      <c r="H5" s="119"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="90"/>
       <c r="J5" s="26"/>
       <c r="L5" s="24"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="99" t="s">
+      <c r="A6" s="71"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="100"/>
-      <c r="H6" s="101"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="104"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="107"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="69"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="93" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="94"/>
-      <c r="H9" s="95"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="98"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="60"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="70" t="s">
+      <c r="A11" s="71"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="110"/>
-      <c r="H11" s="111"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="77"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="114"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="80"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="93" t="s">
+      <c r="A13" s="71"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="95"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="98"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="60"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="49">
+      <c r="A15" s="70">
         <v>2</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="49">
+      <c r="C15" s="93"/>
+      <c r="D15" s="70">
         <v>13</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="55" t="s">
+      <c r="E15" s="49"/>
+      <c r="F15" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="56"/>
-      <c r="H15" s="57"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="96"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="70" t="s">
+      <c r="A16" s="71"/>
+      <c r="B16" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="60"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="99"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="63"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="102"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="64" t="s">
+      <c r="A18" s="71"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="105"/>
       <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="69"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="108"/>
       <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="78" t="s">
+      <c r="A20" s="71"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="79"/>
-      <c r="H20" s="80"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="111"/>
       <c r="I20" s="25"/>
     </row>
     <row r="21" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="83"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="114"/>
       <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="64" t="s">
+      <c r="A22" s="71"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="103" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="65"/>
-      <c r="H22" s="66"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="105"/>
       <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="69"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="108"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="84" t="s">
+      <c r="A24" s="71"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="115" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="85"/>
-      <c r="H24" s="86"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="117"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="72"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="87" t="s">
+      <c r="A25" s="71"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="118" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="88"/>
-      <c r="H25" s="89"/>
+      <c r="G25" s="119"/>
+      <c r="H25" s="120"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="87" t="s">
+      <c r="A26" s="72"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="118" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="88"/>
-      <c r="H26" s="89"/>
+      <c r="G26" s="119"/>
+      <c r="H26" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A15:A26"/>
+    <mergeCell ref="D15:D26"/>
+    <mergeCell ref="E15:E26"/>
+    <mergeCell ref="F15:H17"/>
+    <mergeCell ref="F18:H19"/>
+    <mergeCell ref="B16:C26"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="F22:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
     <mergeCell ref="E3:E14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="F2:H2"/>
@@ -3097,18 +3145,6 @@
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="D3:D14"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="D15:D26"/>
-    <mergeCell ref="E15:E26"/>
-    <mergeCell ref="F15:H17"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="B16:C26"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F20:H21"/>
-    <mergeCell ref="F22:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3119,11 +3155,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
@@ -3132,45 +3168,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="109"/>
+      <c r="C2" s="74"/>
       <c r="D2" s="33" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="92"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="122">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="95" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="56"/>
+      <c r="C3" s="95"/>
       <c r="F3" t="s">
         <v>135</v>
       </c>
@@ -3325,4 +3361,67 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>